<commit_message>
Opportunity pom,excel and test
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/opportunities.xlsx
+++ b/src/main/resources/excel/opportunities.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cools\git\AutoDesk_job1\src\main\resources\excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8300F7BA-669E-4204-9BC5-C803129A9838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="3420" yWindow="3420" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Create" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,8 +24,40 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>Bosch</t>
+  </si>
+  <si>
+    <t>Sales Stage</t>
+  </si>
+  <si>
+    <t>Qualification</t>
+  </si>
+  <si>
+    <t>Campaign Source</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User Conference</t>
+  </si>
+  <si>
+    <t>Sales Subject</t>
+  </si>
+  <si>
+    <t>SO_tiger</t>
+  </si>
+  <si>
+    <t>Sales qty</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -330,13 +368,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.5546875" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
5 testcases , pom and excel
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/opportunities.xlsx
+++ b/src/main/resources/excel/opportunities.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cools\git\AutoDesk_job1\src\main\resources\excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8300F7BA-669E-4204-9BC5-C803129A9838}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3420" yWindow="3420" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="18090" windowHeight="5700"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" r:id="rId1"/>
+    <sheet name="Edit" sheetId="2" r:id="rId2"/>
+    <sheet name="Search" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="124519"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,40 +21,67 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Opportunity Name</t>
   </si>
   <si>
-    <t>Bosch</t>
-  </si>
-  <si>
-    <t>Sales Stage</t>
-  </si>
-  <si>
-    <t>Qualification</t>
-  </si>
-  <si>
-    <t>Campaign Source</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> User Conference</t>
-  </si>
-  <si>
-    <t>Sales Subject</t>
-  </si>
-  <si>
-    <t>SO_tiger</t>
-  </si>
-  <si>
-    <t>Sales qty</t>
+    <t>Related To</t>
+  </si>
+  <si>
+    <t>bosch</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Marketing group</t>
+  </si>
+  <si>
+    <t>Advance search</t>
+  </si>
+  <si>
+    <t>Another DropDown</t>
+  </si>
+  <si>
+    <t>does not contains</t>
+  </si>
+  <si>
+    <t>Opportunity name</t>
+  </si>
+  <si>
+    <t>Opportunity No</t>
+  </si>
+  <si>
+    <t>ends with</t>
+  </si>
+  <si>
+    <t>search text box</t>
+  </si>
+  <si>
+    <t>starts with</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Document Title </t>
+  </si>
+  <si>
+    <t>Pancard</t>
+  </si>
+  <si>
+    <t>File path</t>
+  </si>
+  <si>
+    <t>D:\pancard.txt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,8 +110,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -149,7 +181,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -184,7 +216,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -361,64 +393,152 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:8" ht="30">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
+    <row r="4" spans="1:8">
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>